<commit_message>
Updating Boxes from px -> %
</commit_message>
<xml_diff>
--- a/log_out.xlsx
+++ b/log_out.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K70"/>
+  <dimension ref="A1:K71"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="I18" sqref="I18"/>
@@ -3289,7 +3289,7 @@
     </row>
     <row r="70">
       <c r="A70" s="2" t="n">
-        <v>44414.39481285757</v>
+        <v>44414.39481285879</v>
       </c>
       <c r="B70" t="inlineStr">
         <is>
@@ -3323,6 +3323,47 @@
         <v>4.09</v>
       </c>
       <c r="K70" t="inlineStr">
+        <is>
+          <t>Tier Summer Pass</t>
+        </is>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" s="2" t="n">
+        <v>44416.82094497623</v>
+      </c>
+      <c r="B71" t="inlineStr">
+        <is>
+          <t>work</t>
+        </is>
+      </c>
+      <c r="C71" t="n">
+        <v>1</v>
+      </c>
+      <c r="D71" t="n">
+        <v>1</v>
+      </c>
+      <c r="E71" t="n">
+        <v>1</v>
+      </c>
+      <c r="F71" t="inlineStr">
+        <is>
+          <t>other2</t>
+        </is>
+      </c>
+      <c r="G71" t="n">
+        <v>0</v>
+      </c>
+      <c r="H71" t="n">
+        <v>0</v>
+      </c>
+      <c r="I71" t="n">
+        <v>0</v>
+      </c>
+      <c r="J71" t="n">
+        <v>4.09</v>
+      </c>
+      <c r="K71" t="inlineStr">
         <is>
           <t>Tier Summer Pass</t>
         </is>

</xml_diff>